<commit_message>
add expord exel and fix css site
</commit_message>
<xml_diff>
--- a/public/file.xlsx
+++ b/public/file.xlsx
@@ -4544,14 +4544,6 @@
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
-  <mergeCells>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A11:C11"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="A34:C34"/>
-  </mergeCells>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1"/>

</xml_diff>